<commit_message>
fixed order of sheets in dav bo
sub-scripted plotting functions

weights side-by side comparison plot sorted
</commit_message>
<xml_diff>
--- a/Data/Delphi round 1/response sheets/Dave Bo - give your expert opinion on woodland condition1114.xlsx
+++ b/Data/Delphi round 1/response sheets/Dave Bo - give your expert opinion on woodland condition1114.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Woodland-condition/Data/Delphi round 1/response sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="697" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69A1912D-95EE-45A9-9EFA-D62662B568B3}"/>
+  <xr:revisionPtr revIDLastSave="698" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98EDD12A-E1FF-43C1-8098-4783D98956A1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree age distribution" sheetId="20" r:id="rId1"/>
     <sheet name="Native canopy percentage " sheetId="4" r:id="rId2"/>
-    <sheet name="N tree &amp; shrub spp." sheetId="5" r:id="rId3"/>
-    <sheet name="Vertical structure" sheetId="9" r:id="rId4"/>
+    <sheet name="Vertical structure" sheetId="9" r:id="rId3"/>
+    <sheet name="N tree &amp; shrub spp." sheetId="5" r:id="rId4"/>
     <sheet name="Invasive plants % cover" sheetId="6" r:id="rId5"/>
     <sheet name="Deadwood" sheetId="10" r:id="rId6"/>
     <sheet name="Veteran trees" sheetId="11" r:id="rId7"/>
@@ -4778,6 +4778,397 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'Vertical structure'!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative value to woodland condition</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Vertical structure'!$A$10:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Vertical structure'!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E077-43FB-81BB-CB021CC0C02C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2030676528"/>
+        <c:axId val="2030676944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2030676528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vertical structure'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of canopy layers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2030676944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2030676944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Example indicator'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative value to woodland condition</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2030676528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1527093014269697"/>
+          <c:y val="8.2687623940269128E-2"/>
+          <c:w val="0.8109105747627382"/>
+          <c:h val="0.71926057238569585"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'N tree &amp; shrub spp.'!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -5017,397 +5408,6 @@
         <c:crossAx val="2030676944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2030676944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Example indicator'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Relative value to woodland condition</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2030676528"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.1527093014269697"/>
-          <c:y val="8.2687623940269128E-2"/>
-          <c:w val="0.8109105747627382"/>
-          <c:h val="0.71926057238569585"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Vertical structure'!$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Relative value to woodland condition</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Vertical structure'!$A$10:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Vertical structure'!$B$10:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>90</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E077-43FB-81BB-CB021CC0C02C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2030676528"/>
-        <c:axId val="2030676944"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2030676528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="4"/>
-          <c:min val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Vertical structure'!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Number of canopy layers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2030676944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2030676944"/>
@@ -16869,7 +16869,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A71B85C5-8AA2-4BB6-B468-EB3648C570AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DFD5C4-1B80-41AA-8F56-CCFDC190784F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16897,8 +16897,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>173935</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>182217</xdr:rowOff>
     </xdr:to>
@@ -16907,7 +16907,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{597A6D94-9F46-4AD6-86C4-C0AA96B072F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F232AB-325B-4C04-A27C-08896F50EAC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16915,8 +16915,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2493065" y="1648239"/>
-          <a:ext cx="3023152" cy="182217"/>
+          <a:off x="2489338" y="1647825"/>
+          <a:ext cx="3237672" cy="182217"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -16968,7 +16968,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DFD5C4-1B80-41AA-8F56-CCFDC190784F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A71B85C5-8AA2-4BB6-B468-EB3648C570AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16996,8 +16996,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>173935</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>182217</xdr:rowOff>
     </xdr:to>
@@ -17006,7 +17006,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F232AB-325B-4C04-A27C-08896F50EAC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{597A6D94-9F46-4AD6-86C4-C0AA96B072F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17014,8 +17014,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2489338" y="1647825"/>
-          <a:ext cx="3237672" cy="182217"/>
+          <a:off x="2493065" y="1648239"/>
+          <a:ext cx="3023152" cy="182217"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -18717,6 +18717,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F115801-BE0C-4AA3-B3C2-4C039C0D91A4}" name="Table15689" displayName="Table15689" ref="A9:B17" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A9:B17" xr:uid="{AB04B7AD-16D4-48B1-9771-A4B9EAE35B9B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:B17">
+    <sortCondition ref="A9:A17"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{645C5C7F-4195-455D-B30B-1C0EDE27E05E}" name="Number of canopy layers" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{AC8FEEF9-AD35-49FF-8F7C-506AD938D0D9}" name="Relative value to woodland condition" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{34E56704-5D90-4D5C-AC12-5904D85A5240}" name="Table156" displayName="Table156" ref="A9:B20" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A9:B20" xr:uid="{AB04B7AD-16D4-48B1-9771-A4B9EAE35B9B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:B19">
@@ -18725,20 +18739,6 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{45980BC9-3E5B-4A4D-A3EF-E1FD5F360097}" name="Number of tree and shrub species" dataDxfId="45"/>
     <tableColumn id="2" xr3:uid="{2893B8B3-F98F-4F27-89AD-13681B4C8CB2}" name="Relative value to woodland condition" dataDxfId="44"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F115801-BE0C-4AA3-B3C2-4C039C0D91A4}" name="Table15689" displayName="Table15689" ref="A9:B17" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A9:B17" xr:uid="{AB04B7AD-16D4-48B1-9771-A4B9EAE35B9B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:B17">
-    <sortCondition ref="A9:A17"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{645C5C7F-4195-455D-B30B-1C0EDE27E05E}" name="Number of canopy layers" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{AC8FEEF9-AD35-49FF-8F7C-506AD938D0D9}" name="Relative value to woodland condition" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -22609,7 +22609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874D2522-2B76-4503-81F6-47499AF8A525}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -23044,6 +23044,527 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADE01BF-891C-4D98-B138-661CC22AFA79}">
+  <dimension ref="A1:R54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:18" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>40</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>80</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="I14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="I16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="I20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="D27" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D10:R11"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="D27:N28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E3BDB2-4936-4583-A0D1-731A826C7FE6}">
   <dimension ref="A1:R54"/>
   <sheetViews>
@@ -23505,527 +24026,6 @@
     <mergeCell ref="D10:R11"/>
     <mergeCell ref="D27:N28"/>
     <mergeCell ref="I14:M14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADE01BF-891C-4D98-B138-661CC22AFA79}">
-  <dimension ref="A1:R54"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>10</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>40</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>80</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="I14" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="I16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="I20" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-    </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="D27" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-    </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="D29" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D10:R11"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="D27:N28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26633,25 +26633,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
-      <UserInfo>
-        <DisplayName>Christine Reid</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>David Bonsall</DisplayName>
-        <AccountId>62</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF102A4A1803344B8D888EB900B09227" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43bc291949bcf5a898aed47fdf38e56c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="090e8724-afd2-4a00-8d2e-c87448cad135" xmlns:ns3="cce065d8-4207-498d-8ddb-77753710233a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a89575b99fa510669e25d545522f68e" ns2:_="" ns3:_="">
     <xsd:import namespace="090e8724-afd2-4a00-8d2e-c87448cad135"/>
@@ -26842,6 +26823,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
+      <UserInfo>
+        <DisplayName>Christine Reid</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>David Bonsall</DisplayName>
+        <AccountId>62</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
   <ds:schemaRefs>
@@ -26851,16 +26851,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6617C3D-29D9-48EE-BF3C-21AA1A387073}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26877,4 +26867,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>